<commit_message>
[add]add auto delete saga instance code
</commit_message>
<xml_diff>
--- a/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-sys-setting.xlsx
+++ b/src/main/resources/script/db/init-data/hzero_platform/hzero_platform/choerodon-sys-setting.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\c7n-hzero\hzero-iam\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projcect\iam\hzero-iam\src\main\resources\script\db\init-data\hzero_platform\hzero_platform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0562FD9F-2970-4602-B9C6-6403C2F96E21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7A949C3-7E5C-4726-BADB-D022F5784B63}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="71">
   <si>
     <r>
       <rPr>
@@ -2066,6 +2066,23 @@
   </si>
   <si>
     <t>autoCleanWebhookRecordInterval</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanSagaInstance</t>
+  </si>
+  <si>
+    <t>FALSE</t>
+    <phoneticPr fontId="23" type="noConversion"/>
+  </si>
+  <si>
+    <t>autoCleanSagaInstanceInterval</t>
+  </si>
+  <si>
+    <t>retainFailedSagaInstance</t>
+  </si>
+  <si>
+    <t>TRUE</t>
     <phoneticPr fontId="23" type="noConversion"/>
   </si>
 </sst>
@@ -2073,7 +2090,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -2227,6 +2244,12 @@
       <family val="2"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF6A8759"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -2366,7 +2389,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2458,6 +2481,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2806,21 +2833,21 @@
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="15.58203125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" style="5" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="28.08203125" customWidth="1"/>
+    <col min="3" max="3" width="28.109375" customWidth="1"/>
     <col min="4" max="4" width="35.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="38.58203125" customWidth="1"/>
-    <col min="6" max="6" width="23.4140625" customWidth="1"/>
-    <col min="7" max="7" width="21.58203125" customWidth="1"/>
+    <col min="5" max="5" width="38.5546875" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5546875" customWidth="1"/>
     <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="24.58203125" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" customWidth="1"/>
     <col min="10" max="10" width="27" customWidth="1"/>
-    <col min="11" max="11" width="19.08203125" customWidth="1"/>
-    <col min="12" max="12" width="18.58203125" customWidth="1"/>
-    <col min="13" max="13" width="13.08203125" customWidth="1"/>
+    <col min="11" max="11" width="19.109375" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="13.109375" customWidth="1"/>
     <col min="14" max="1025" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2835,7 +2862,7 @@
       <c r="G1" s="22"/>
       <c r="H1" s="22"/>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="18">
       <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:8" ht="49.5" customHeight="1">
@@ -2849,7 +2876,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="18">
       <c r="C4" s="41" t="s">
         <v>3</v>
       </c>
@@ -2870,7 +2897,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="18">
       <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
@@ -2890,7 +2917,7 @@
       </c>
       <c r="E8" s="27"/>
     </row>
-    <row r="9" spans="1:8" ht="52.2">
+    <row r="9" spans="1:8" ht="51.75">
       <c r="C9" s="13" t="s">
         <v>13</v>
       </c>
@@ -2904,7 +2931,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="52.2">
+    <row r="10" spans="1:8" ht="51.75">
       <c r="C10" s="15" t="s">
         <v>17</v>
       </c>
@@ -2915,7 +2942,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="69.599999999999994">
+    <row r="11" spans="1:8" ht="69">
       <c r="C11" s="11" t="s">
         <v>20</v>
       </c>
@@ -2947,7 +2974,7 @@
       <c r="D14" s="12"/>
       <c r="E14" s="27"/>
     </row>
-    <row r="15" spans="1:8" ht="34.799999999999997">
+    <row r="15" spans="1:8" ht="34.5">
       <c r="C15" s="16" t="s">
         <v>26</v>
       </c>
@@ -2970,7 +2997,7 @@
       <c r="D19" s="42"/>
       <c r="E19" s="42"/>
     </row>
-    <row r="20" spans="3:5">
+    <row r="20" spans="3:5" ht="18">
       <c r="C20" s="18" t="s">
         <v>31</v>
       </c>
@@ -2978,7 +3005,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="21" spans="3:5">
+    <row r="21" spans="3:5" ht="18">
       <c r="C21" s="18" t="s">
         <v>33</v>
       </c>
@@ -2986,7 +3013,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="22" spans="3:5">
+    <row r="22" spans="3:5" ht="18">
       <c r="C22" s="18" t="s">
         <v>35</v>
       </c>
@@ -2994,7 +3021,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="3:5">
+    <row r="23" spans="3:5" ht="18">
       <c r="C23" s="18" t="s">
         <v>37</v>
       </c>
@@ -3020,7 +3047,7 @@
       </c>
       <c r="E26" s="38"/>
     </row>
-    <row r="27" spans="3:5" ht="52.2">
+    <row r="27" spans="3:5" ht="51.75">
       <c r="C27" s="21" t="s">
         <v>43</v>
       </c>
@@ -3043,20 +3070,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.399999999999999"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.25"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="8.4140625" customWidth="1"/>
-    <col min="4" max="4" width="12.25" customWidth="1"/>
+    <col min="1" max="1" width="16.21875" customWidth="1"/>
+    <col min="2" max="2" width="8.44140625" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="21.33203125" customWidth="1"/>
-    <col min="9" max="9" width="21.08203125" customWidth="1"/>
+    <col min="9" max="9" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -3196,6 +3223,39 @@
         <v>180</v>
       </c>
     </row>
+    <row r="15" spans="1:7">
+      <c r="E15" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="E16" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F16" s="43" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="32">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="17" spans="5:7">
+      <c r="E17" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="F17" s="43" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>70</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="23" type="noConversion"/>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>